<commit_message>
Update: - remove DSM section by campaign - add new Reconfirm format
</commit_message>
<xml_diff>
--- a/src/main/resources/config/template/exportKpiTemplate.xlsx
+++ b/src/main/resources/config/template/exportKpiTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780"/>
   </bookViews>
   <sheets>
     <sheet name="BY_CAMPAIGN" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Position</t>
   </si>
@@ -304,7 +304,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -327,12 +327,7 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -356,19 +351,30 @@
     <xf numFmtId="10" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="2" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="3" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -667,19 +673,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="3.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5703125" style="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.28515625" customWidth="1"/>
     <col min="10" max="10" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -707,7 +713,7 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="27"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3" t="s">
         <v>7</v>
@@ -717,28 +723,28 @@
       </c>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
+      <c r="A2" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6">
+        <v>22</v>
+      </c>
+      <c r="C2" s="40">
         <v>0</v>
       </c>
       <c r="D2" s="7">
         <v>0</v>
       </c>
       <c r="E2" s="17">
-        <v>9870300</v>
-      </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2" s="26">
-        <v>0</v>
-      </c>
-      <c r="H2" s="28"/>
+        <v>0</v>
+      </c>
+      <c r="F2" s="42">
+        <v>0</v>
+      </c>
+      <c r="G2" s="43">
+        <v>0</v>
+      </c>
+      <c r="H2" s="25"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
         <v>12</v>
@@ -750,24 +756,18 @@
     <row r="3" spans="1:11">
       <c r="A3" s="10"/>
       <c r="B3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>0</v>
-      </c>
-      <c r="E3" s="18">
-        <v>0.15</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="26">
-        <v>0</v>
-      </c>
-      <c r="H3" s="29"/>
+        <v>23</v>
+      </c>
+      <c r="C3" s="41"/>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0</v>
+      </c>
+      <c r="F3" s="42"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="26"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3" t="s">
         <v>15</v>
@@ -777,26 +777,26 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="10"/>
+      <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6">
         <v>0</v>
       </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="18">
-        <v>0.88</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="26">
-        <v>0</v>
-      </c>
-      <c r="H4" s="29"/>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="35">
+        <v>0</v>
+      </c>
+      <c r="G4" s="23">
+        <v>0</v>
+      </c>
+      <c r="H4" s="26"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3" t="s">
         <v>11</v>
@@ -808,89 +808,97 @@
     <row r="5" spans="1:11">
       <c r="A5" s="10"/>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
       </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="18">
-        <v>0.5</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="26">
-        <v>0</v>
-      </c>
-      <c r="H5" s="29"/>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="34">
+        <v>0</v>
+      </c>
+      <c r="F5" s="35">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0</v>
+      </c>
+      <c r="H5" s="26"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="33"/>
-      <c r="B6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="14">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="15">
-        <v>0</v>
-      </c>
-      <c r="H6" s="29"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="35">
+        <v>0</v>
+      </c>
+      <c r="F6" s="35">
+        <v>0</v>
+      </c>
+      <c r="G6" s="23">
+        <v>0</v>
+      </c>
+      <c r="H6" s="26"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="35">
-        <v>0</v>
-      </c>
-      <c r="D7" s="7">
-        <v>0</v>
-      </c>
-      <c r="E7" s="17">
-        <v>0</v>
-      </c>
-      <c r="F7" s="37">
-        <v>0</v>
-      </c>
-      <c r="G7" s="38">
-        <v>0</v>
-      </c>
-      <c r="H7" s="28"/>
+      <c r="A7" s="30">
+        <v>1234567</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="14">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="15">
+        <v>0</v>
+      </c>
+      <c r="H7" s="25"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="10"/>
+      <c r="A8" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="36"/>
+        <v>10</v>
+      </c>
+      <c r="C8" s="39">
+        <v>0.25</v>
+      </c>
       <c r="D8" s="7">
         <v>0</v>
       </c>
       <c r="E8" s="17">
-        <v>0</v>
-      </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="28"/>
+        <v>150000</v>
+      </c>
+      <c r="F8" s="35">
+        <v>0</v>
+      </c>
+      <c r="G8" s="23">
+        <v>0</v>
+      </c>
+      <c r="H8" s="25"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -898,24 +906,24 @@
     <row r="9" spans="1:11">
       <c r="A9" s="1"/>
       <c r="B9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="11">
-        <v>0</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0</v>
-      </c>
-      <c r="G9" s="26">
-        <v>0</v>
-      </c>
-      <c r="H9" s="29"/>
+        <v>26</v>
+      </c>
+      <c r="C9" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="34">
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="F9" s="35">
+        <v>0</v>
+      </c>
+      <c r="G9" s="23">
+        <v>0</v>
+      </c>
+      <c r="H9" s="26"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -923,24 +931,24 @@
     <row r="10" spans="1:11">
       <c r="A10" s="10"/>
       <c r="B10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="D10" s="11">
-        <v>0</v>
-      </c>
-      <c r="E10" s="18">
-        <v>0</v>
-      </c>
-      <c r="F10" s="8">
-        <v>0</v>
-      </c>
-      <c r="G10" s="26">
-        <v>0</v>
-      </c>
-      <c r="H10" s="29"/>
+        <v>27</v>
+      </c>
+      <c r="C10" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="37">
+        <v>0</v>
+      </c>
+      <c r="E10" s="36">
+        <v>75</v>
+      </c>
+      <c r="F10" s="35">
+        <v>0</v>
+      </c>
+      <c r="G10" s="23">
+        <v>0</v>
+      </c>
+      <c r="H10" s="26"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
@@ -948,36 +956,34 @@
     <row r="11" spans="1:11">
       <c r="A11" s="10"/>
       <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="11">
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <v>0</v>
-      </c>
-      <c r="F11" s="8">
-        <v>0</v>
-      </c>
-      <c r="G11" s="26">
-        <v>0</v>
-      </c>
-      <c r="H11" s="29"/>
+        <v>14</v>
+      </c>
+      <c r="C11" s="39">
+        <v>0.25</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="34">
+        <v>0.88717948717948714</v>
+      </c>
+      <c r="F11" s="35">
+        <v>0</v>
+      </c>
+      <c r="G11" s="23">
+        <v>0</v>
+      </c>
+      <c r="H11" s="26"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="33">
-        <v>1234567</v>
-      </c>
+      <c r="A12" s="30"/>
       <c r="B12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="38">
         <v>1</v>
       </c>
       <c r="D12" s="3"/>
@@ -986,137 +992,46 @@
       <c r="G12" s="15">
         <v>0</v>
       </c>
-      <c r="H12" s="29"/>
+      <c r="H12" s="26"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="20">
-        <v>0</v>
-      </c>
-      <c r="D13" s="7">
-        <v>0</v>
-      </c>
-      <c r="E13" s="17">
-        <v>150000</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0</v>
-      </c>
-      <c r="G13" s="26">
-        <v>0</v>
-      </c>
-      <c r="H13" s="28"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="1"/>
-      <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="20">
-        <v>0</v>
-      </c>
-      <c r="D14" s="11">
-        <v>0</v>
-      </c>
-      <c r="E14" s="18">
-        <v>0.90909090909090906</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="26">
-        <v>0</v>
-      </c>
-      <c r="H14" s="29"/>
+      <c r="H14" s="26"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="10"/>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="20">
-        <v>0</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="17">
-        <v>75</v>
-      </c>
-      <c r="F15" s="8">
-        <v>0</v>
-      </c>
-      <c r="G15" s="26">
-        <v>0</v>
-      </c>
-      <c r="H15" s="29"/>
+      <c r="H15" s="26"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="10"/>
-      <c r="B16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="20">
-        <v>0</v>
-      </c>
-      <c r="D16" s="11">
-        <v>0</v>
-      </c>
-      <c r="E16" s="18">
-        <v>0.88717948717948714</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="26">
-        <v>0</v>
-      </c>
-      <c r="H16" s="29"/>
+      <c r="H16" s="26"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="33"/>
-      <c r="B17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="21">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="15">
-        <v>0</v>
-      </c>
-      <c r="H17" s="29"/>
+    <row r="17" spans="8:11">
+      <c r="H17" s="26"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1128,14 +1043,14 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
     <col min="7" max="7" width="8.85546875" customWidth="1"/>
@@ -1182,10 +1097,10 @@
       <c r="E2" s="17">
         <v>9870300</v>
       </c>
-      <c r="F2" s="8">
-        <v>0</v>
-      </c>
-      <c r="G2" s="26">
+      <c r="F2" s="35">
+        <v>0</v>
+      </c>
+      <c r="G2" s="23">
         <v>0</v>
       </c>
       <c r="H2" s="9" t="s">
@@ -1200,16 +1115,16 @@
       <c r="C3" s="6">
         <v>0.2</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="33">
         <v>0.75</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="34">
         <v>0.90909090909090906</v>
       </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="26">
+      <c r="F3" s="35">
+        <v>0</v>
+      </c>
+      <c r="G3" s="23">
         <v>0</v>
       </c>
       <c r="H3" s="8"/>
@@ -1222,16 +1137,16 @@
       <c r="C4" s="6">
         <v>0.1</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="33">
         <v>0.85</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="34">
         <v>0.79</v>
       </c>
-      <c r="F4" s="8">
-        <v>0</v>
-      </c>
-      <c r="G4" s="26">
+      <c r="F4" s="35">
+        <v>0</v>
+      </c>
+      <c r="G4" s="23">
         <v>0</v>
       </c>
       <c r="H4" s="8"/>
@@ -1244,17 +1159,17 @@
       <c r="C5" s="6">
         <v>0.1</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="35">
         <v>0.2</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="34">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="F5" s="8">
-        <v>0</v>
-      </c>
-      <c r="G5" s="26">
+      <c r="F5" s="35">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23">
         <v>0</v>
       </c>
       <c r="H5" s="8"/>
@@ -1284,7 +1199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1311,37 +1226,37 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="15.75">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="22"/>
     </row>
     <row r="4" spans="1:5" ht="15.75">
-      <c r="A4" s="39"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="25"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12"/>
       <c r="B5" s="13"/>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="31" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>